<commit_message>
add prerequisites code, and no info for empty fields
</commit_message>
<xml_diff>
--- a/DataScrapping/scraped_courses.xlsx
+++ b/DataScrapping/scraped_courses.xlsx
@@ -1,97 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/WongKang/Documents/js tutorial/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B1B820-7AC5-C642-A95C-5B8498B3A800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>course_id</t>
-  </si>
-  <si>
-    <t>course_title</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>terms_available</t>
-  </si>
-  <si>
-    <t>course_lead</t>
-  </si>
-  <si>
-    <t>course_lead_info</t>
-  </si>
-  <si>
-    <t>pillar</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>02.121DH</t>
-  </si>
-  <si>
-    <t>The Question of Being</t>
-  </si>
-  <si>
-    <t>This course is centered on the question of being. What do we mean when we say that something “is”? Or more abstractly, what is being? This question has been at the center of philosophical enquiry since the inception of Greek thought, and is the basis upon which Plato’s and later Aristotle’s speculations developed, which then served as an unavoidable point of reference and confrontation for any subsequent thinker. The question regarding being and the possibility of knowing it through our mental categories is the backbone of Western philosophy. For, it is on the basis of this question that the concept of truth as “adequation of thing and intellect” has been shaped in Western philosophical tradition. This particular understanding of what truth is finds its inceptions in Aristotle’s investigation of being to then reach its most mature formulation at the dawn of modern philosophy: it is then that the reciprocal relation of man to being as one of subject to objects comes to the fore. This concept of truth has since Descartes served and still serves as the ground for the sciences and their approach to reality. The 20th century, however, has seen a challenging questioning of the subject-objects relation of man to being as handed down by tradition: the works of Martin Heidegger represent a provoking re-proposition of the question of being and hence of the question of the essence of truth. Is the relation between man and being reducible to the scheme of subject-objects? What does it mean to truly know what being is? This course aims at guiding the students through the history of this central question – “what is being?” – which, given its pivotal role in the subsequent development of Western thought, can serve as an introduction to the history of philosophy specifically, while more generally at the same time as an opportunity to pose some questions regarding the understanding of reality that guides our techno-scientifically minded world.</t>
-  </si>
-  <si>
-    <t>[4, 6, 8]</t>
-  </si>
-  <si>
-    <t>Paolo Di Leo</t>
-  </si>
-  <si>
-    <t>https://www.sutd.edu.sg/profile/paolo-di-leo/</t>
-  </si>
-  <si>
-    <t>HASS</t>
-  </si>
-  <si>
-    <t>Elective / Technical Elective</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -106,46 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -433,73 +420,485 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>course_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>course_title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>terms_available</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>course_lead</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>course_lead_info</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>pillar</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>prerequisites</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>prerequisites_links</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="312" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>02.121DH</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>The Question of Being</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>This course is centered on the question of being. What do we mean when we say that something “is”? Or more abstractly, what is being? This question has been at the center of philosophical enquiry since the inception of Greek thought, and is the basis upon which Plato’s and later Aristotle’s speculations developed, which then served as an unavoidable point of reference and confrontation for any subsequent thinker. The question regarding being and the possibility of knowing it through our mental categories is the backbone of Western philosophy. For, it is on the basis of this question that the concept of truth as “adequation of thing and intellect” has been shaped in Western philosophical tradition. This particular understanding of what truth is finds its inceptions in Aristotle’s investigation of being to then reach its most mature formulation at the dawn of modern philosophy: it is then that the reciprocal relation of man to being as one of subject to objects comes to the fore. This concept of truth has since Descartes served and still serves as the ground for the sciences and their approach to reality. The 20th century, however, has seen a challenging questioning of the subject-objects relation of man to being as handed down by tradition: the works of Martin Heidegger represent a provoking re-proposition of the question of being and hence of the question of the essence of truth. Is the relation between man and being reducible to the scheme of subject-objects? What does it mean to truly know what being is? This course aims at guiding the students through the history of this central question – “what is being?” – which, given its pivotal role in the subsequent development of Western thought, can serve as an introduction to the history of philosophy specifically, while more generally at the same time as an opportunity to pose some questions regarding the understanding of reality that guides our techno-scientifically minded world.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[4, 6, 8]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Paolo Di Leo</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.sutd.edu.sg/profile/paolo-di-leo/</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>HASS</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Elective / Technical Elective</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>['no info']</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>['no info']</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>40.002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Optimisation</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>The course covers a broad range of optimisation algorithms and models. The course will cover the following topics: linear programming, simplex algorithm, duality, sensitivity analysis, two player zero-sum games, network optimisation, minimum cost flow, network simplex algorithm, integer programming, branch and bound methods, cutting plane methods, dynamic programming. Throughout the course, a number of applications from various areas will be discussed.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[4]</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ESD</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>['10.018 Modelling Space and Systems']</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>['https://www.sutd.edu.sg/course/10-018-modelling-space-and-systems']</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>40.011</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Data and Business Analytics</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>This course provides an introduction to the Engineering Systems and Design pillar by focusing on using industrial or commercial data to identify an opportunity for system improvement and estimating the value of this improvement to the system owner. A signature feature of the course and the primary motivation for the course material comes from a team-based, semester-long project for an external client. Students develop skills in organising industrial projects and in presenting their results in oral, written, and poster form. In addition, problems in improving system throughput and flowtime are used throughout to motivate many of the topics. Students acquire skills in data manipulation, data visualisation, data analysis, system modelling, revenue and cost estimation, financial ratio analysis, and business simulation.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[4]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ESD</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>['10.014 Computational Thinking for Design', '10.022 Modelling Uncertainty']</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>['https://www.sutd.edu.sg/course/10-014-computational-thinking-for-design/', 'https://www.sutd.edu.sg/course/10-022-modelling-uncertainty/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>40.017</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Probability and Statistics</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>This course builds upon the material taught in Modelling Uncertainty. The course will provide students with the foundations of data analysis, and give them tools for analyzing situations that involve uncertainty and building statistical models. It will also develop students’ critical thinking skills. Applications and examples relevant to engineering systems will be given. The topics covered will include: multivariate normal, Poisson process, limit theorems, regression, point and interval estimation, hypothesis testing, analysis of variance, and introductory Bayesian statistics.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[4]</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ESD</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>['10.018 Modelling Space and Systems', '10.022 Modelling Uncertainty']</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>['https://www.sutd.edu.sg/course/10-018-modelling-space-and-systems/', 'https://www.sutd.edu.sg/course/10-022-modelling-uncertainty/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>40.012</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Manufacturing and Service Operations</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>This course introduces concepts and techniques related to the design, planning, control, and improvement of both manufacturing and service systems. The course provides basic definitions of operations management terms, tools and techniques for analysing system operations, and a strategic context for making operational decisions. In particular, the topics covered include: Manufacturing and inventory decisions for single and multi-echelon systems under deterministic and stochastic demand in the presence or absence of production/transportation lead time; trade-off between fixed cost of production and inventory holding costs; trade-off between holding and back-order/stock-out costs; stochastic modelling and queuing analysis for analysing transient and steady-state performance of service systems; cost analysis of multi-server queues and network of queues; priority queues; risk pooling in manufacturing and service systems.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[5]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ESD</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>['40.002 Optimisation', '40.017 Probability &amp; Statistics']</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>['https://www.sutd.edu.sg/course/40-002-optimisation/', 'https://www.sutd.edu.sg/course/40-017-probability-and-statistics/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>40.014</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Engineering Systems Architecture</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>This course is no longer offered after 2024.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>[5]</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>ESD</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>['40.011 Data and Business Analytics', '40.002 Optimisation']</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>['https://www.sutd.edu.sg/course/40-011-data-and-business-analytics-for-esd-students-only/', 'https://www.sutd.edu.sg/course/40-002-optimisation/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>40.016</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>The Analytics Edge</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>The increasing availability of data is changing the way organizations are thinking about themselves and the way they interact with the world. Data is helping improve the profits of businesses, the quality of life of individuals, the predictions on performance of sports teams and social interactions. In this course you will learn how to use data and analytics to give you an edge. The course will expose students to real world examples of how analytics is being used with examples from Moneyball, Watson and the Framingham Heart Study among others. Through these examples you will learn on how to use tools of analytics such as linear regression, logistic regression, classification and regression trees, graphical models, visualization, text analytics, clustering and optimization in practice. The statistical software R and spreadsheets will be used in the course.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>[5]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>ESD</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>['40.017 Probability and Statistics', '10.022 Modelling Uncertainty']</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>['https://www.sutd.edu.sg/course/40-017-probability-and-statistics/', 'https://www.sutd.edu.sg/course/10-022-modelling-uncertainty/']</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>40.018</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Heuristics and Systems Theory</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Iterative methods are mathematical procedures that use an initial value to generate a sequence of improving approximate solutions for a class of problems, in which the current approximation is derived from the previous ones. This course introduces two important types of iterative methodologies often encountered in the analysis and design of engineering systems: 1) metaheuristic optimisation algorithms; and 2) model-based analysis and design tools for dynamical systems.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>[5]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>no info</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>ESD</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>['10.018 Modelling Space and Systems', '40.002 Optimisation', '40.017 Probability and Statistics']</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>['https://www.sutd.edu.sghttps://www.sutd.edu.sg/course/10-018-modelling-space-and-systems', 'https://www.sutd.edu.sghttps://www.sutd.edu.sg/course/40-002-optimisation', 'https://www.sutd.edu.sghttps://www.sutd.edu.sg/course/40-017-probability-and-statistics']</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>